<commit_message>
set a data model and upload method for offline
</commit_message>
<xml_diff>
--- a/Mott_doc/mott_APIList_v2.xlsx
+++ b/Mott_doc/mott_APIList_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Accord\Mott\Mott\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\mottMacDonald\Mott_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="23010" windowHeight="10095" tabRatio="500"/>
+    <workbookView xWindow="2970" yWindow="0" windowWidth="23010" windowHeight="10095" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,12 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
@@ -512,6 +506,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -869,124 +869,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.625" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="6"/>
+    <col min="1" max="1" width="11.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="13"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="str">
+      <c r="B7" s="11" t="str">
         <f>CONCATENATE(B2,B5)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getAllContract</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="str">
+      <c r="B12" s="11" t="str">
         <f>CONCATENATE($B$2,B10)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getAllTemplates</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="13" t="str">
+      <c r="B17" s="11" t="str">
         <f>CONCATENATE($B$2,B15)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getConditionOptions</v>
       </c>
@@ -995,31 +995,31 @@
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="13" t="str">
+      <c r="B22" s="11" t="str">
         <f>CONCATENATE($B$2,B20)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getHumidityOptions</v>
       </c>
@@ -1028,31 +1028,31 @@
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="13" t="str">
+      <c r="B27" s="11" t="str">
         <f>CONCATENATE($B$2,B25)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getWindOptions</v>
       </c>
@@ -1061,31 +1061,31 @@
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="13" t="str">
+      <c r="B32" s="11" t="str">
         <f>CONCATENATE($B$2,B30)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/getAnswerOptions</v>
       </c>
@@ -1094,48 +1094,48 @@
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="13" t="str">
+      <c r="B37" s="11" t="str">
         <f>CONCATENATE($B$2,B35)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/saveFormInfo</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+    <row r="39" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1143,48 +1143,48 @@
       <c r="A40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="13" t="str">
+      <c r="B44" s="11" t="str">
         <f>CONCATENATE($B$2,B42)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/saveFormWeather</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1192,45 +1192,45 @@
       <c r="A47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="13" t="str">
+      <c r="B51" s="11" t="str">
         <f>CONCATENATE($B$2,B49)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/saveFormItem</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -1246,43 +1246,43 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="13" t="str">
+      <c r="B58" s="11" t="str">
         <f>CONCATENATE($B$2,B56)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/saveFormItemObservation</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="11" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1290,48 +1290,48 @@
       <c r="A61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="13" t="str">
+      <c r="B65" s="11" t="str">
         <f>CONCATENATE($B$2,B63)</f>
         <v>http://mott.accordhkdev.com/api/v1/api/api.php?p=mapi/saveFormItems</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="12" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>